<commit_message>
Correction to entry update
</commit_message>
<xml_diff>
--- a/entries.xlsx
+++ b/entries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thana\Documents\Resume-Builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB87A29D-3B7A-4608-B564-A183BC15A53D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A30E5B8-59BB-481E-BF8B-F96BF1BB897D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="870" yWindow="4350" windowWidth="24090" windowHeight="15435" tabRatio="671" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -499,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -562,9 +562,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="17" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1066,7 +1063,7 @@
   <dimension ref="A1:I1002"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1122,10 +1119,12 @@
       <c r="D2" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="E2" s="30">
+      <c r="E2" s="29">
         <v>44105</v>
       </c>
-      <c r="F2" s="29"/>
+      <c r="F2" s="29">
+        <v>44166</v>
+      </c>
       <c r="G2" s="27" t="s">
         <v>126</v>
       </c>

</xml_diff>